<commit_message>
Organizado os Projetos do Intensivao de Python
</commit_message>
<xml_diff>
--- a/Projetos/03 - Automação Web e Busca de Informações/commodities_atualizado.xlsx
+++ b/Projetos/03 - Automação Web e Busca de Informações/commodities_atualizado.xlsx
@@ -441,7 +441,7 @@
         <v>85.31999999999999</v>
       </c>
       <c r="C2">
-        <v>85.23999999999999</v>
+        <v>68.68000000000001</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -455,7 +455,7 @@
         <v>163.59</v>
       </c>
       <c r="C3">
-        <v>160.78</v>
+        <v>133.17</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -469,7 +469,7 @@
         <v>282.2</v>
       </c>
       <c r="C4">
-        <v>278.9</v>
+        <v>279.15</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -483,7 +483,7 @@
         <v>424.37</v>
       </c>
       <c r="C5">
-        <v>382.63</v>
+        <v>392.46</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
@@ -497,7 +497,7 @@
         <v>497.76</v>
       </c>
       <c r="C6">
-        <v>480</v>
+        <v>410.01</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -511,10 +511,10 @@
         <v>136.23</v>
       </c>
       <c r="C7">
-        <v>135.68</v>
+        <v>147.82</v>
       </c>
       <c r="D7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -525,10 +525,10 @@
         <v>1092.87</v>
       </c>
       <c r="C8">
-        <v>1113.46</v>
+        <v>1092.76</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -539,7 +539,7 @@
         <v>321.77</v>
       </c>
       <c r="C9">
-        <v>338.43</v>
+        <v>324.22</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
@@ -553,7 +553,7 @@
         <v>1549.11</v>
       </c>
       <c r="C10">
-        <v>1548.7</v>
+        <v>0</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -567,10 +567,10 @@
         <v>9.050000000000001</v>
       </c>
       <c r="C11">
-        <v>9.050000000000001</v>
+        <v>9.609999999999999</v>
       </c>
       <c r="D11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>